<commit_message>
Added practice feature, not yet optimal
</commit_message>
<xml_diff>
--- a/amino_acids/resources/AA_data.xlsx
+++ b/amino_acids/resources/AA_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeromlu2\LukaFiles\04_Programiranje\01_Python\02_MyProjects\Amino_acids\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeromlu2\LukaFiles\01_Programming\01_Python\02_MyProjects\aminoacids\amino_acids\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="amino_acids" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">amino_acids!$A$2:$N$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">amino_acids!$A$2:$O$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,8 +26,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Jeromel, Luka</author>
+  </authors>
+  <commentList>
+    <comment ref="O2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jeromel, Luka:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Measure of hydrophobic effect. High positive value means strong hidrophobicity.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="112">
   <si>
     <t>Amino_acid</t>
   </si>
@@ -360,13 +394,16 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>Hydropathy index</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -380,6 +417,19 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -695,14 +745,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K23" sqref="K23"/>
+      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -717,7 +767,7 @@
     <col min="14" max="14" width="31.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
@@ -733,7 +783,7 @@
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
     </row>
-    <row r="2" spans="1:14" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>69</v>
       </c>
@@ -774,8 +824,11 @@
       <c r="N2" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O2" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -815,8 +868,11 @@
       <c r="N3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O3">
+        <v>-4.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -856,8 +912,11 @@
       <c r="N4" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4">
+        <v>-3.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -900,8 +959,11 @@
       <c r="N5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5">
+        <v>-3.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -941,8 +1003,11 @@
       <c r="N6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O6">
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -982,8 +1047,11 @@
       <c r="N7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7">
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1017,8 +1085,11 @@
       <c r="N8" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1055,8 +1126,11 @@
       <c r="N9" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9">
+        <v>-0.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1093,8 +1167,11 @@
       <c r="N10" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O10">
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1131,8 +1208,11 @@
       <c r="N11" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O11">
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1172,8 +1252,11 @@
       <c r="N12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O12">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1214,7 +1297,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1251,8 +1334,11 @@
       <c r="N14" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O14">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1289,8 +1375,11 @@
       <c r="N15" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O15">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1330,8 +1419,11 @@
       <c r="N16" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O16">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1371,8 +1463,11 @@
       <c r="N17" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O17">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1412,8 +1507,11 @@
       <c r="N18" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O18">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1453,8 +1551,11 @@
       <c r="N19" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O19">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1494,8 +1595,11 @@
       <c r="N20" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O20">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1538,8 +1642,11 @@
       <c r="N21" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O21">
+        <v>-1.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1579,8 +1686,11 @@
       <c r="N22" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O22">
+        <v>-0.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1620,8 +1730,11 @@
       <c r="N23" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O23">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1639,15 +1752,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:N2">
-    <sortState ref="A3:N24">
-      <sortCondition ref="A2"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A2:O2"/>
   <mergeCells count="1">
     <mergeCell ref="K1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>